<commit_message>
files/hl7/excel-templates: Update excel templates
Signed-off-by: Ariel D'Alessandro <ariel.dalessandro@gmail.com>
</commit_message>
<xml_diff>
--- a/files/hl7/excel-templates/Laboratorio Canino.xlsx
+++ b/files/hl7/excel-templates/Laboratorio Canino.xlsx
@@ -19,12 +19,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Bioquímica!$A$1:$M$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hemograma!$A$1:$M$46</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="99">
   <si>
     <t>Paciente:</t>
   </si>
@@ -303,6 +303,24 @@
   </si>
   <si>
     <t>V.R.: 125 - 250 mg/dL</t>
+  </si>
+  <si>
+    <t>${paciente}</t>
+  </si>
+  <si>
+    <t>${sexo}</t>
+  </si>
+  <si>
+    <t>${edad}</t>
+  </si>
+  <si>
+    <t>${responsable}</t>
+  </si>
+  <si>
+    <t>${fecha}</t>
+  </si>
+  <si>
+    <t>${solicita}</t>
   </si>
 </sst>
 </file>
@@ -608,21 +626,39 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -643,34 +679,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -685,8 +697,14 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1076,8 +1094,8 @@
       <xdr:rowOff>185057</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>673701</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3141</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>22591</xdr:rowOff>
     </xdr:to>
@@ -1385,15 +1403,15 @@
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F4" s="1"/>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
     </row>
     <row r="5" spans="1:28" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -1401,15 +1419,15 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="58" t="s">
+      <c r="G5" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -1426,15 +1444,15 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="7"/>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="60"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -1451,15 +1469,15 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="G7" s="61" t="s">
+      <c r="G7" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -1476,15 +1494,15 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -1521,22 +1539,26 @@
     </row>
     <row r="10" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="62" t="s">
+      <c r="C10" s="57"/>
+      <c r="D10" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="62"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="66"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="56"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
@@ -1555,22 +1577,26 @@
     </row>
     <row r="11" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
       <c r="G11" s="63" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="63"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="68"/>
+      <c r="I11" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="66"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
@@ -1589,22 +1615,26 @@
     </row>
     <row r="12" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
       <c r="G12" s="64" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="64"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="70"/>
+      <c r="I12" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="68"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -1653,12 +1683,12 @@
     </row>
     <row r="14" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
       <c r="F14" s="18"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -1685,12 +1715,12 @@
     </row>
     <row r="15" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
       <c r="F15" s="21"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -1748,11 +1778,11 @@
     <row r="17" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="24"/>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
       <c r="F17" s="25" t="s">
         <v>26</v>
       </c>
@@ -1761,12 +1791,12 @@
       </c>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
@@ -1786,23 +1816,23 @@
     <row r="18" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
       <c r="F18" s="26"/>
       <c r="G18" s="11" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
-      <c r="J18" s="46" t="s">
+      <c r="J18" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
@@ -1822,11 +1852,11 @@
     <row r="19" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="11" t="s">
         <v>27</v>
       </c>
@@ -1835,12 +1865,12 @@
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
-      <c r="J19" s="46" t="s">
+      <c r="J19" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
@@ -1860,11 +1890,11 @@
     <row r="20" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="11" t="s">
         <v>28</v>
       </c>
@@ -1873,12 +1903,12 @@
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
-      <c r="J20" s="46" t="s">
+      <c r="J20" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="46"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
@@ -1897,12 +1927,12 @@
     </row>
     <row r="21" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -1930,11 +1960,11 @@
     <row r="22" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
       <c r="F22" s="11" t="s">
         <v>29</v>
       </c>
@@ -1943,12 +1973,12 @@
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
-      <c r="J22" s="46" t="s">
+      <c r="J22" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
@@ -1968,11 +1998,11 @@
     <row r="23" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
       <c r="F23" s="11" t="s">
         <v>30</v>
       </c>
@@ -1981,12 +2011,12 @@
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
-      <c r="J23" s="46" t="s">
+      <c r="J23" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
@@ -2035,20 +2065,20 @@
     </row>
     <row r="25" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
@@ -2067,20 +2097,20 @@
     </row>
     <row r="26" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="71"/>
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
@@ -2129,12 +2159,12 @@
     </row>
     <row r="28" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27"/>
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
       <c r="F28" s="11"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
@@ -2174,12 +2204,12 @@
         <v>13</v>
       </c>
       <c r="H29" s="11"/>
-      <c r="J29" s="46" t="s">
+      <c r="J29" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
@@ -2230,21 +2260,21 @@
     <row r="31" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
       <c r="F31" s="11" t="s">
         <v>58</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="47" t="s">
+      <c r="H31" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="I31" s="47"/>
+      <c r="I31" s="49"/>
       <c r="J31" s="11" t="e">
         <f>$F$29*F31/100</f>
         <v>#VALUE!</v>
@@ -2252,10 +2282,10 @@
       <c r="K31" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L31" s="50" t="s">
+      <c r="L31" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="M31" s="50"/>
+      <c r="M31" s="47"/>
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
@@ -2275,19 +2305,19 @@
     <row r="32" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="46" t="s">
+      <c r="C32" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="47" t="s">
+      <c r="H32" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="I32" s="47"/>
+      <c r="I32" s="49"/>
       <c r="J32" s="11" t="e">
         <f t="shared" ref="J32:J35" si="0">$F$29*F32/100</f>
         <v>#VALUE!</v>
@@ -2295,10 +2325,10 @@
       <c r="K32" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L32" s="50" t="s">
+      <c r="L32" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="M32" s="50"/>
+      <c r="M32" s="47"/>
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
       <c r="P32" s="9"/>
@@ -2318,21 +2348,21 @@
     <row r="33" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
       <c r="F33" s="11" t="s">
         <v>59</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="47" t="s">
+      <c r="H33" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="I33" s="47"/>
+      <c r="I33" s="49"/>
       <c r="J33" s="11" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -2340,10 +2370,10 @@
       <c r="K33" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L33" s="50" t="s">
+      <c r="L33" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="M33" s="50"/>
+      <c r="M33" s="47"/>
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
@@ -2363,21 +2393,21 @@
     <row r="34" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
       <c r="F34" s="11" t="s">
         <v>60</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="47" t="s">
+      <c r="H34" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="I34" s="47"/>
+      <c r="I34" s="49"/>
       <c r="J34" s="11" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -2385,10 +2415,10 @@
       <c r="K34" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L34" s="50" t="s">
+      <c r="L34" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="M34" s="50"/>
+      <c r="M34" s="47"/>
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
@@ -2408,19 +2438,19 @@
     <row r="35" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="46" t="s">
+      <c r="C35" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="47" t="s">
+      <c r="H35" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="I35" s="47"/>
+      <c r="I35" s="49"/>
       <c r="J35" s="11" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -2428,10 +2458,10 @@
       <c r="K35" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L35" s="50" t="s">
+      <c r="L35" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="M35" s="50"/>
+      <c r="M35" s="47"/>
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
@@ -2480,20 +2510,20 @@
     </row>
     <row r="37" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="71"/>
+      <c r="M37" s="71"/>
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
@@ -2512,20 +2542,20 @@
     </row>
     <row r="38" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="71"/>
+      <c r="M38" s="71"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
@@ -2574,11 +2604,11 @@
     </row>
     <row r="40" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27"/>
-      <c r="B40" s="71" t="s">
+      <c r="B40" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="71"/>
-      <c r="D40" s="71"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="9"/>
       <c r="F40" s="11"/>
       <c r="G40" s="9"/>
@@ -2607,23 +2637,23 @@
     <row r="41" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
-      <c r="C41" s="46" t="s">
+      <c r="C41" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11" t="s">
         <v>20</v>
       </c>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
-      <c r="J41" s="46" t="s">
+      <c r="J41" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="K41" s="46"/>
-      <c r="L41" s="46"/>
-      <c r="M41" s="46"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="45"/>
+      <c r="M41" s="45"/>
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
@@ -2643,11 +2673,11 @@
     <row r="42" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
-      <c r="C42" s="46" t="s">
+      <c r="C42" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
       <c r="F42" s="11" t="s">
         <v>32</v>
       </c>
@@ -2656,12 +2686,12 @@
       </c>
       <c r="H42" s="11"/>
       <c r="I42" s="11"/>
-      <c r="J42" s="46" t="s">
+      <c r="J42" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="K42" s="46"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="46"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="45"/>
+      <c r="M42" s="45"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
@@ -2712,20 +2742,20 @@
     </row>
     <row r="44" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="46"/>
-      <c r="M44" s="46"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="45"/>
+      <c r="L44" s="45"/>
+      <c r="M44" s="45"/>
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
       <c r="P44" s="9"/>
@@ -2744,20 +2774,20 @@
     </row>
     <row r="45" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="46"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="45"/>
+      <c r="M45" s="45"/>
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
       <c r="P45" s="9"/>
@@ -2776,20 +2806,20 @@
     </row>
     <row r="46" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="46"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="45"/>
+      <c r="L46" s="45"/>
+      <c r="M46" s="45"/>
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
       <c r="P46" s="9"/>
@@ -6265,6 +6295,58 @@
     <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="F38:M38"/>
+    <mergeCell ref="F44:M44"/>
+    <mergeCell ref="F45:M45"/>
+    <mergeCell ref="F46:M46"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="F37:M37"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="F25:M25"/>
+    <mergeCell ref="F26:M26"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
     <mergeCell ref="B46:E46"/>
     <mergeCell ref="G8:M8"/>
     <mergeCell ref="L33:M33"/>
@@ -6281,58 +6363,6 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C19:E19"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="F25:M25"/>
-    <mergeCell ref="F26:M26"/>
-    <mergeCell ref="F38:M38"/>
-    <mergeCell ref="F44:M44"/>
-    <mergeCell ref="F45:M45"/>
-    <mergeCell ref="F46:M46"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="F37:M37"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F46:M46">
@@ -6391,15 +6421,15 @@
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F4" s="1"/>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
     </row>
     <row r="5" spans="1:28" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -6407,15 +6437,15 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="58" t="s">
+      <c r="G5" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -6432,15 +6462,15 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="7"/>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="60"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -6457,15 +6487,15 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="G7" s="61" t="s">
+      <c r="G7" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -6482,15 +6512,15 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -6527,22 +6557,26 @@
     </row>
     <row r="10" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="62" t="s">
+      <c r="C10" s="57"/>
+      <c r="D10" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="62"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="66"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="56"/>
       <c r="N10" s="34"/>
       <c r="O10" s="34"/>
       <c r="P10" s="34"/>
@@ -6561,22 +6595,26 @@
     </row>
     <row r="11" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
       <c r="G11" s="63" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="63"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="68"/>
+      <c r="I11" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="66"/>
       <c r="N11" s="34"/>
       <c r="O11" s="34"/>
       <c r="P11" s="34"/>
@@ -6595,22 +6633,26 @@
     </row>
     <row r="12" spans="1:28" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
       <c r="G12" s="64" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="64"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="70"/>
+      <c r="I12" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="68"/>
       <c r="N12" s="34"/>
       <c r="O12" s="34"/>
       <c r="P12" s="34"/>
@@ -10122,21 +10164,6 @@
     <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:M12"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="G10:H10"/>
@@ -10146,6 +10173,21 @@
     <mergeCell ref="G6:M6"/>
     <mergeCell ref="G7:M7"/>
     <mergeCell ref="G8:M8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J19:M19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:M26">

</xml_diff>